<commit_message>
Re-Run Stats + Tidy Up DiCE/SHAP
</commit_message>
<xml_diff>
--- a/Experiment Output/Feb/Post Scale Rerun/PostStabilityRuns/Format/ANCHOR_XAI_Metrics_Experiments.xlsx
+++ b/Experiment Output/Feb/Post Scale Rerun/PostStabilityRuns/Format/ANCHOR_XAI_Metrics_Experiments.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TU_D\Dissertation\Dissertation_PreWork\Experiment Output\Feb\Post Scale Rerun\PostStabilityRuns\Format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\T_UD\Dissertation\PreWork_Repo\Dissertation_PreWork\Experiment Output\Feb\Post Scale Rerun\PostStabilityRuns\Format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E55E0DB-8786-47CC-B653-06132D9EE5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C991E7-F132-4C1B-84B0-42C831DAC892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="630" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-4815" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sample Number</t>
   </si>
@@ -39,13 +52,16 @@
   <si>
     <t>Comp_Efficiency</t>
   </si>
+  <si>
+    <t>Mean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -237,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -260,12 +276,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,24 +585,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G22"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -605,7 +622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -625,7 +642,7 @@
         <v>2650.621102571487</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="6">
         <v>2</v>
       </c>
@@ -645,7 +662,7 @@
         <v>2442.143568515778</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="6">
         <v>3</v>
       </c>
@@ -665,7 +682,7 @@
         <v>2648.7332680225368</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="6">
         <v>4</v>
       </c>
@@ -685,7 +702,7 @@
         <v>2399.271505594254</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="6">
         <v>5</v>
       </c>
@@ -705,7 +722,7 @@
         <v>2490.101202249527</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="6">
         <v>6</v>
       </c>
@@ -725,7 +742,7 @@
         <v>2680.834575414658</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="6">
         <v>7</v>
       </c>
@@ -745,7 +762,7 @@
         <v>2633.8235049247742</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" s="6">
         <v>8</v>
       </c>
@@ -765,7 +782,7 @@
         <v>2552.8997800350189</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="6">
         <v>9</v>
       </c>
@@ -785,7 +802,7 @@
         <v>2718.1416850090031</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" s="6">
         <v>10</v>
       </c>
@@ -805,7 +822,7 @@
         <v>2703.427858114243</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" s="6">
         <v>11</v>
       </c>
@@ -825,7 +842,7 @@
         <v>2547.7510919570918</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B14" s="6">
         <v>12</v>
       </c>
@@ -845,7 +862,7 @@
         <v>2810.4390864372249</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="6">
         <v>13</v>
       </c>
@@ -865,7 +882,7 @@
         <v>2522.4007570743561</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="6">
         <v>14</v>
       </c>
@@ -885,7 +902,7 @@
         <v>2608.0894327163701</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="6">
         <v>15</v>
       </c>
@@ -905,7 +922,7 @@
         <v>2695.1234216690059</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="6">
         <v>16</v>
       </c>
@@ -925,7 +942,7 @@
         <v>2886.646767854691</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="6">
         <v>17</v>
       </c>
@@ -945,7 +962,7 @@
         <v>2843.9518961906429</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="6">
         <v>18</v>
       </c>
@@ -965,7 +982,7 @@
         <v>2727.806860685349</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="6">
         <v>19</v>
       </c>
@@ -985,7 +1002,7 @@
         <v>2530.8348257541661</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="7">
         <v>20</v>
       </c>
@@ -1003,6 +1020,31 @@
       </c>
       <c r="G22" s="12">
         <v>2933.1400127410889</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="14">
+        <f>AVERAGE(C3:C22)</f>
+        <v>11.09375</v>
+      </c>
+      <c r="D25" s="14">
+        <f t="shared" ref="D25:G25" si="0">AVERAGE(D3:D22)</f>
+        <v>52.578125</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="shared" si="0"/>
+        <v>2.265625</v>
+      </c>
+      <c r="F25" s="14">
+        <f t="shared" si="0"/>
+        <v>1.7667723912057085</v>
+      </c>
+      <c r="G25" s="14">
+        <f t="shared" si="0"/>
+        <v>2651.3091101765631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>